<commit_message>
update big cyl steeper motor
</commit_message>
<xml_diff>
--- a/引脚使用.xlsx
+++ b/引脚使用.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\封片机\Glass_Package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC4A3DF-D208-4FF0-BC52-ABA829194F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D66778-21B4-4BB8-B9A4-781A28999211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6510" yWindow="2445" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1201,10 +1201,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>GOH_mid_sensor</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>G</t>
     </r>
@@ -1239,23 +1235,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>G</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OV_glass_sensor</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>GP_sucker_sensor</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1409,6 +1388,27 @@
   </si>
   <si>
     <t>ITV0011电源开关</t>
+  </si>
+  <si>
+    <t>GOV_glass_sensor</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P_big_cyl_sensor</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1932,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView tabSelected="1" topLeftCell="C82" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1944,6 +1944,7 @@
     <col min="5" max="5" width="26.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.375" style="2" customWidth="1"/>
     <col min="7" max="7" width="21.625" customWidth="1"/>
+    <col min="8" max="8" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.15">
@@ -1993,7 +1994,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.15">
@@ -2205,7 +2206,7 @@
         <v>58</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.15">
@@ -2480,7 +2481,7 @@
         <v>113</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.15">
@@ -2498,7 +2499,7 @@
         <v>116</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.15">
@@ -2533,7 +2534,7 @@
         <v>123</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.15">
@@ -2548,10 +2549,10 @@
         <v>126</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.15">
@@ -2569,7 +2570,7 @@
         <v>129</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.15">
@@ -2659,7 +2660,7 @@
         <v>144</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.15">
@@ -2677,7 +2678,7 @@
         <v>147</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.15">
@@ -2751,7 +2752,7 @@
         <v>160</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.15">
@@ -2808,7 +2809,7 @@
         <v>172</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.15">
@@ -2826,7 +2827,7 @@
         <v>175</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.15">
@@ -2844,7 +2845,7 @@
         <v>178</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.15">
@@ -2862,7 +2863,7 @@
         <v>181</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.15">
@@ -2880,7 +2881,7 @@
         <v>184</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.15">
@@ -2898,7 +2899,7 @@
         <v>187</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.15">
@@ -2916,7 +2917,7 @@
         <v>190</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.15">
@@ -2924,7 +2925,7 @@
         <v>191</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="4" t="s">
@@ -2934,7 +2935,7 @@
         <v>192</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.15">
@@ -3228,7 +3229,7 @@
         <v>258</v>
       </c>
       <c r="G82" s="15" t="s">
-        <v>340</v>
+        <v>369</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.15">
@@ -3243,10 +3244,10 @@
         <v>261</v>
       </c>
       <c r="F83" s="22" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H83" s="15"/>
     </row>
@@ -3280,7 +3281,7 @@
         <v>269</v>
       </c>
       <c r="G85" s="15" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.15">
@@ -3298,7 +3299,7 @@
         <v>273</v>
       </c>
       <c r="G86" s="15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.15">
@@ -3316,7 +3317,7 @@
         <v>277</v>
       </c>
       <c r="G87" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.15">
@@ -3334,7 +3335,7 @@
         <v>281</v>
       </c>
       <c r="G88" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.15">
@@ -3351,8 +3352,9 @@
       <c r="F89" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="G89" s="15" t="s">
-        <v>343</v>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.15">
@@ -3403,7 +3405,7 @@
         <v>294</v>
       </c>
       <c r="F92" s="18" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G92" s="15"/>
     </row>
@@ -3498,10 +3500,10 @@
         <v>315</v>
       </c>
       <c r="F98" s="18" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
update glass out process
</commit_message>
<xml_diff>
--- a/引脚使用.xlsx
+++ b/引脚使用.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\封片机\Glass_Package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D66778-21B4-4BB8-B9A4-781A28999211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4730D9D8-2BA1-4B4F-826D-B6E3AE6EDF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="2445" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1394,20 +1394,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>G</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P_big_cyl_sensor</t>
-    </r>
+    <t>GP_cyl_pos_sensor</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1932,7 +1919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C82" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C70" workbookViewId="0">
       <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
@@ -3352,10 +3339,10 @@
       <c r="F89" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="G89" s="15"/>
-      <c r="H89" s="15" t="s">
+      <c r="G89" s="15" t="s">
         <v>370</v>
       </c>
+      <c r="H89" s="15"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B90" s="6" t="s">

</xml_diff>